<commit_message>
Levels for sort data frame
</commit_message>
<xml_diff>
--- a/Data/results_survey_relecov_bioinfo.xlsx
+++ b/Data/results_survey_relecov_bioinfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="results_survey_relecov_bioinfo" sheetId="1" state="visible" r:id="rId2"/>
@@ -1125,7 +1125,7 @@
     <t xml:space="preserve">COD_2104</t>
   </si>
   <si>
-    <t xml:space="preserve">Instituto Tecnológico y de Energías Renovables, S.A.</t>
+    <t xml:space="preserve">Instituto Tecnológico y de Energías Renovables</t>
   </si>
   <si>
     <t xml:space="preserve">COD_2111</t>
@@ -1262,8 +1262,8 @@
   </sheetPr>
   <dimension ref="A1:AZ19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4118,16 +4118,16 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="66.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="42.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
   </cols>
@@ -4481,7 +4481,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="68.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="4" style="0" width="66.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="126.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="111"/>

</xml_diff>